<commit_message>
created line chart with population numbers across the state over time
</commit_message>
<xml_diff>
--- a/wireframe/data/poverty_allyears.xlsx
+++ b/wireframe/data/poverty_allyears.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Documents/github/epkh.github.io/wireframe/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phoebe/Documents/github/epkh.github.io/wireframe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="23140" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="4000" yWindow="460" windowWidth="23140" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>WGTP</t>
   </si>
@@ -57,6 +57,27 @@
   </si>
   <si>
     <t>OWNERS</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>renterpov</t>
+  </si>
+  <si>
+    <t>ownerpov</t>
+  </si>
+  <si>
+    <t>burden50r</t>
+  </si>
+  <si>
+    <t>burden50h</t>
+  </si>
+  <si>
+    <t>burden30r</t>
+  </si>
+  <si>
+    <t>burden30h</t>
   </si>
 </sst>
 </file>
@@ -438,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="L1" sqref="L1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,7 +470,7 @@
     <col min="6" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -462,8 +483,29 @@
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2">
         <v>2005</v>
@@ -478,8 +520,35 @@
         <f>D2/C2</f>
         <v>0.25876417269957497</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>2005</v>
+      </c>
+      <c r="K2">
+        <f>D2</f>
+        <v>346604</v>
+      </c>
+      <c r="L2">
+        <f>D13</f>
+        <v>201420</v>
+      </c>
+      <c r="M2">
+        <f>E7</f>
+        <v>204191</v>
+      </c>
+      <c r="N2">
+        <f>E18</f>
+        <v>127869</v>
+      </c>
+      <c r="O2">
+        <f>D7</f>
+        <v>250498</v>
+      </c>
+      <c r="P2">
+        <f>D18</f>
+        <v>166345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3">
         <v>2010</v>
@@ -494,8 +563,35 @@
         <f>D3/C3</f>
         <v>0.24381487570273339</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>2010</v>
+      </c>
+      <c r="K3">
+        <f>D3</f>
+        <v>307443</v>
+      </c>
+      <c r="L3">
+        <f>D14</f>
+        <v>200467</v>
+      </c>
+      <c r="M3">
+        <f>E8</f>
+        <v>232912</v>
+      </c>
+      <c r="N3">
+        <f>E19</f>
+        <v>119445</v>
+      </c>
+      <c r="O3">
+        <f>D8</f>
+        <v>281238</v>
+      </c>
+      <c r="P3">
+        <f>D19</f>
+        <v>155151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4">
         <v>2015</v>
@@ -510,11 +606,38 @@
         <f>D4/C4</f>
         <v>0.23689768153637455</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>2015</v>
+      </c>
+      <c r="K4">
+        <f>D4</f>
+        <v>338089</v>
+      </c>
+      <c r="L4">
+        <f>D15</f>
+        <v>191255</v>
+      </c>
+      <c r="M4">
+        <f>E9</f>
+        <v>219648</v>
+      </c>
+      <c r="N4">
+        <f>E20</f>
+        <v>121062</v>
+      </c>
+      <c r="O4">
+        <f>D9</f>
+        <v>267391</v>
+      </c>
+      <c r="P4">
+        <f>D20</f>
+        <v>151350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="C6" s="4" t="s">
         <v>0</v>
@@ -532,7 +655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7">
         <v>2005</v>
@@ -555,7 +678,7 @@
         <v>0.71069924471824863</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8">
         <v>2010</v>
@@ -578,7 +701,7 @@
         <v>0.7388941586272314</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9">
         <v>2015</v>
@@ -601,7 +724,7 @@
         <v>0.72401483312731763</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -615,7 +738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13">
         <v>2005</v>
@@ -631,7 +754,7 @@
         <v>5.8416507202150351E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14">
         <v>2010</v>
@@ -647,7 +770,7 @@
         <v>5.8284355270369084E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15">
         <v>2015</v>
@@ -663,7 +786,7 @@
         <v>5.6536480965809995E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>